<commit_message>
basic 2-Dim Arrray example 6.3.4EKMEDJE
</commit_message>
<xml_diff>
--- a/docs/inf-A93-ZADANIA.xlsx
+++ b/docs/inf-A93-ZADANIA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3150" windowWidth="21570" windowHeight="11235"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="21570" windowHeight="11235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>MM</t>
   </si>
@@ -55,12 +55,15 @@
   <si>
     <t>BLOKove</t>
   </si>
+  <si>
+    <t>Z6 - LOOPs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +75,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -255,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -278,14 +290,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,45 +584,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="18">
         <f>C2/80</f>
-        <v>10.492291666666667</v>
-      </c>
-      <c r="B2" s="20">
+        <v>19.402708333333333</v>
+      </c>
+      <c r="B2" s="18">
         <f>C2/45</f>
-        <v>18.652962962962963</v>
-      </c>
-      <c r="C2" s="20">
-        <f>SUM(C5+C13+C24+C69+C81)+(D2/60)</f>
-        <v>839.38333333333333</v>
-      </c>
-      <c r="D2" s="21">
-        <f>SUM(D5+D24+D69+D81)</f>
-        <v>1283</v>
+        <v>34.493703703703702</v>
+      </c>
+      <c r="C2" s="18">
+        <f>SUM(C5+C13+C24+C69+C81+C83)+(D2/60)</f>
+        <v>1552.2166666666667</v>
+      </c>
+      <c r="D2" s="19">
+        <f>SUM(D5+D24+D69+D81++C81+C83)</f>
+        <v>1993</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -671,10 +689,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="9">
@@ -751,10 +769,10 @@
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="23"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C24" s="16">
@@ -1103,10 +1121,10 @@
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D68" s="18"/>
+      <c r="D68" s="23"/>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" s="17">
@@ -1191,10 +1209,10 @@
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D80" s="18"/>
+      <c r="D80" s="20"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81">
@@ -1204,14 +1222,279 @@
         <v>0</v>
       </c>
     </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="21"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="1">
+        <f>SUM(C84:C114)</f>
+        <v>701</v>
+      </c>
+      <c r="D83" s="1">
+        <f>SUM(D84:D114)</f>
+        <v>793</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>6</v>
+      </c>
+      <c r="D85">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>9</v>
+      </c>
+      <c r="D88">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <v>9</v>
+      </c>
+      <c r="D89">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>3</v>
+      </c>
+      <c r="D90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>7</v>
+      </c>
+      <c r="D91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>14</v>
+      </c>
+      <c r="D92">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>50</v>
+      </c>
+      <c r="D95">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>44</v>
+      </c>
+      <c r="D96">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>7</v>
+      </c>
+      <c r="D97">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>41</v>
+      </c>
+      <c r="D99">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>44</v>
+      </c>
+      <c r="D100">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <v>41</v>
+      </c>
+      <c r="D101">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>60</v>
+      </c>
+      <c r="D102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>37</v>
+      </c>
+      <c r="D103">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>29</v>
+      </c>
+      <c r="D105">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>24</v>
+      </c>
+      <c r="D106">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>31</v>
+      </c>
+      <c r="D107">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>40</v>
+      </c>
+      <c r="D108">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>58</v>
+      </c>
+      <c r="D109">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>5</v>
+      </c>
+      <c r="D110">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>32</v>
+      </c>
+      <c r="D111">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <v>21</v>
+      </c>
+      <c r="D112">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <v>42</v>
+      </c>
+      <c r="D113">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>11</v>
+      </c>
+      <c r="D114">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C82:D82"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C80:D80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>